<commit_message>
Added Music List Template.
</commit_message>
<xml_diff>
--- a/WorshipCreator.TestData/Source/Books/CcliTop100/CcliTop100.xlsx
+++ b/WorshipCreator.TestData/Source/Books/CcliTop100/CcliTop100.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PageOptimizer\Data\WorshipCreator.TestData\Source\Books\CcliTop100\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E512764C-1C9C-4964-A614-23053FF0350B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06632916-C13B-4981-B5C6-055AEC3B70B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8764540B-17CA-4663-B848-BB803B99CCC3}"/>
+    <workbookView minimized="1" xWindow="5280" yWindow="4245" windowWidth="21600" windowHeight="11505" firstSheet="5" activeTab="10" xr2:uid="{8764540B-17CA-4663-B848-BB803B99CCC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CcliCombined" sheetId="5" r:id="rId1"/>
@@ -20,10 +20,14 @@
     <sheet name="PraiseChartsTop100AllTime" sheetId="4" r:id="rId5"/>
     <sheet name="MultiTracksTop120" sheetId="6" r:id="rId6"/>
     <sheet name="MultiTracksTop120Global" sheetId="7" r:id="rId7"/>
+    <sheet name="Top100HymnsBBC" sheetId="8" r:id="rId8"/>
+    <sheet name="Top100HymnsPopularHymns" sheetId="9" r:id="rId9"/>
+    <sheet name="Top100HymnsJWPepper" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet4" sheetId="11" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CcliCombined!$A$1:$H$196</definedName>
@@ -33,6 +37,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">MultiTracksTop120!$A$1:$F$121</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">MultiTracksTop120Global!$A$1:$F$121</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">PraiseChartsTop100AllTime!$A$1:$H$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Sheet4!$A$1:$B$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Top100HymnsBBC!$A$1:$B$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2973" uniqueCount="931">
   <si>
     <t>Way Maker</t>
   </si>
@@ -1784,6 +1790,1068 @@
   </si>
   <si>
     <t>MultiTracksTop120Global</t>
+  </si>
+  <si>
+    <t>https://www.bbc.co.uk/programmes/articles/42TSJ0LNMfp0h0wNvxqlw93/2013-the-uks-top-100-hymns</t>
+  </si>
+  <si>
+    <t>https://popularhymns.com/top100</t>
+  </si>
+  <si>
+    <t>A Mighty Fortress Is Our God</t>
+  </si>
+  <si>
+    <t>Abide With Me</t>
+  </si>
+  <si>
+    <t>Alas And Did My Savior Bleed?</t>
+  </si>
+  <si>
+    <t>All Creatures of our God and King</t>
+  </si>
+  <si>
+    <t>All Hail The Power of Jesus' Name</t>
+  </si>
+  <si>
+    <t>All The Way My Savior Leads Me</t>
+  </si>
+  <si>
+    <t>Amazing Grace</t>
+  </si>
+  <si>
+    <t>Are You Washed in the Blood?</t>
+  </si>
+  <si>
+    <t>At Calvary</t>
+  </si>
+  <si>
+    <t>Battle Hymn of the Republic</t>
+  </si>
+  <si>
+    <t>Be Thou My Vision</t>
+  </si>
+  <si>
+    <t>Before The Throne of God Above</t>
+  </si>
+  <si>
+    <t>Blessed Assurance</t>
+  </si>
+  <si>
+    <t>Blest Be The Tie That Binds</t>
+  </si>
+  <si>
+    <t>Child of the King</t>
+  </si>
+  <si>
+    <t>Christ The Lord Is Risen Today</t>
+  </si>
+  <si>
+    <t>Cleanse Me</t>
+  </si>
+  <si>
+    <t>Come Thou Fount of Every Blessing</t>
+  </si>
+  <si>
+    <t>Count Your Blessings</t>
+  </si>
+  <si>
+    <t>Crown Him With Many Crowns</t>
+  </si>
+  <si>
+    <t>Day By Day</t>
+  </si>
+  <si>
+    <t>Doxology</t>
+  </si>
+  <si>
+    <t>Eternal Father, Strong To Save</t>
+  </si>
+  <si>
+    <t>Face To Face</t>
+  </si>
+  <si>
+    <t>Fairest Lord Jesus</t>
+  </si>
+  <si>
+    <t>Faith is the Victory</t>
+  </si>
+  <si>
+    <t>Faith of our Fathers</t>
+  </si>
+  <si>
+    <t>Fight the Good Fight</t>
+  </si>
+  <si>
+    <t>God Leads His Dear Children Along</t>
+  </si>
+  <si>
+    <t>God Will Take Care Of You</t>
+  </si>
+  <si>
+    <t>Guide Me, O Thou Great Jehovah</t>
+  </si>
+  <si>
+    <t>Hark! The Herald Angels Sing</t>
+  </si>
+  <si>
+    <t>Have Thine Own Way, Lord</t>
+  </si>
+  <si>
+    <t>He Hideth My Soul</t>
+  </si>
+  <si>
+    <t>He Is Coming Again</t>
+  </si>
+  <si>
+    <t>He Lives</t>
+  </si>
+  <si>
+    <t>His Eye Is On the Sparrow</t>
+  </si>
+  <si>
+    <t>Holy, Holy, Holy</t>
+  </si>
+  <si>
+    <t>How Firm A Foundation</t>
+  </si>
+  <si>
+    <t>I Am Thine, O Lord</t>
+  </si>
+  <si>
+    <t>I Love To Tell The Story</t>
+  </si>
+  <si>
+    <t>I Need Thee Ev'ry Hour</t>
+  </si>
+  <si>
+    <t>I Surrender All</t>
+  </si>
+  <si>
+    <t>I'd Rather Have Jesus</t>
+  </si>
+  <si>
+    <t>I'll Fly Away</t>
+  </si>
+  <si>
+    <t>In the Garden</t>
+  </si>
+  <si>
+    <t>In The Hour of Trial</t>
+  </si>
+  <si>
+    <t>In The Sweet By and By</t>
+  </si>
+  <si>
+    <t>It is Well</t>
+  </si>
+  <si>
+    <t>Jesus, Lover Of My Soul</t>
+  </si>
+  <si>
+    <t>Jesus Loves Me</t>
+  </si>
+  <si>
+    <t>Just As I Am</t>
+  </si>
+  <si>
+    <t>Leaning on the Everlasting Arms</t>
+  </si>
+  <si>
+    <t>Lord I'm Coming Home</t>
+  </si>
+  <si>
+    <t>Love Divine, All Loves Excelling</t>
+  </si>
+  <si>
+    <t>Love Lifted Me</t>
+  </si>
+  <si>
+    <t>Moment By Moment</t>
+  </si>
+  <si>
+    <t>More Love To Thee</t>
+  </si>
+  <si>
+    <t>Morning Has Broken</t>
+  </si>
+  <si>
+    <t>My Faith Looks Up To Thee</t>
+  </si>
+  <si>
+    <t>Nearer My God, To Thee</t>
+  </si>
+  <si>
+    <t>No One Ever Cared for Me Like Jesus</t>
+  </si>
+  <si>
+    <t>Now We Thank All Our God</t>
+  </si>
+  <si>
+    <t>O For A Thousand Tongues To Sing</t>
+  </si>
+  <si>
+    <t>O Little Town of Bethlehem</t>
+  </si>
+  <si>
+    <t>O Worship The King</t>
+  </si>
+  <si>
+    <t>Old Time Religion</t>
+  </si>
+  <si>
+    <t>Pass Me Not, O Gentle Savior</t>
+  </si>
+  <si>
+    <t>Peace, Perfect Peace</t>
+  </si>
+  <si>
+    <t>Praise Him! Praise Him!</t>
+  </si>
+  <si>
+    <t>Precious Lord Take My Hand</t>
+  </si>
+  <si>
+    <t>Rescue The Perishing</t>
+  </si>
+  <si>
+    <t>Revive Us Again</t>
+  </si>
+  <si>
+    <t>Rock of Ages</t>
+  </si>
+  <si>
+    <t>Safe in the Arms of Jesus</t>
+  </si>
+  <si>
+    <t>Saviour, Like a Shepherd Lead Us</t>
+  </si>
+  <si>
+    <t>Softly And Tenderly Jesus Is Calling</t>
+  </si>
+  <si>
+    <t>Standing on the Promises</t>
+  </si>
+  <si>
+    <t>Take My Life and Let It Be</t>
+  </si>
+  <si>
+    <t>Take Time To Be Holy</t>
+  </si>
+  <si>
+    <t>The Old Rugged Cross</t>
+  </si>
+  <si>
+    <t>There Is A Fountain</t>
+  </si>
+  <si>
+    <t>There Is Power In The Blood</t>
+  </si>
+  <si>
+    <t>Till The Storm Passes By</t>
+  </si>
+  <si>
+    <t>Turn Your Eyes Upon Jesus</t>
+  </si>
+  <si>
+    <t>Trust And Obey</t>
+  </si>
+  <si>
+    <t>What A Day That Will Be</t>
+  </si>
+  <si>
+    <t>What A Friend We Have in Jesus</t>
+  </si>
+  <si>
+    <t>What Child Is This?</t>
+  </si>
+  <si>
+    <t>When I Survey The Wondrous Cross</t>
+  </si>
+  <si>
+    <t>When The Roll Is Called Up Yonder</t>
+  </si>
+  <si>
+    <t>When We All Get To Heaven</t>
+  </si>
+  <si>
+    <t>Wherever He Leads, I'll Go</t>
+  </si>
+  <si>
+    <t>Yesterday, Today, Forever</t>
+  </si>
+  <si>
+    <t>A MIGHTY FORTRESS IS OUR GOD</t>
+  </si>
+  <si>
+    <t>ABIDE WITH ME</t>
+  </si>
+  <si>
+    <t>ALL CREATURES OF OUR GOD AND KING</t>
+  </si>
+  <si>
+    <t>ALL HAIL THE POWER OF JESUS NAME</t>
+  </si>
+  <si>
+    <t>AMAZING GRACE</t>
+  </si>
+  <si>
+    <t>AND CAN IT BE</t>
+  </si>
+  <si>
+    <t>ARE YOU WASHED IN THE BLOOD</t>
+  </si>
+  <si>
+    <t>AT THE CROSS</t>
+  </si>
+  <si>
+    <t>BE THOU MY VISION</t>
+  </si>
+  <si>
+    <t>BECAUSE HE LIVES</t>
+  </si>
+  <si>
+    <t>BLESS THE LORD O MY SOUL</t>
+  </si>
+  <si>
+    <t>BLESSED ASSURANCE</t>
+  </si>
+  <si>
+    <t>BREATHE ON ME BREATH OF GOD</t>
+  </si>
+  <si>
+    <t>CHRIST THE LORD IS RISEN TODAY</t>
+  </si>
+  <si>
+    <t>COME THOU ALMIGHTY KING</t>
+  </si>
+  <si>
+    <t>COME THOU FOUNT OF EVERY BLESSING</t>
+  </si>
+  <si>
+    <t>COUNT YOUR BLESSINGS</t>
+  </si>
+  <si>
+    <t>CROWN HIM WITH MANY CROWNS</t>
+  </si>
+  <si>
+    <t>DOWN AT THE CROSS</t>
+  </si>
+  <si>
+    <t>DOXOLOGY</t>
+  </si>
+  <si>
+    <t>FAIREST LORD JESUS</t>
+  </si>
+  <si>
+    <t>FATHER I ADORE YOU</t>
+  </si>
+  <si>
+    <t>GLORIFY THY NAME</t>
+  </si>
+  <si>
+    <t>GOD WILL TAKE CARE OF YOU</t>
+  </si>
+  <si>
+    <t>GRACE GREATER THAN OUR SIN</t>
+  </si>
+  <si>
+    <t>GREAT IS THY FAITHFULNESS</t>
+  </si>
+  <si>
+    <t>HALLELUJAH WHAT A SAVIOR</t>
+  </si>
+  <si>
+    <t>HAVE THINE OWN WAY LORD</t>
+  </si>
+  <si>
+    <t>HE HIDETH MY SOUL</t>
+  </si>
+  <si>
+    <t>HE KEEPS ME SINGING</t>
+  </si>
+  <si>
+    <t>HE LIVES</t>
+  </si>
+  <si>
+    <t>HEAVEN CAME DOWN</t>
+  </si>
+  <si>
+    <t>HE'S GOT THE WHOLE WORLD IN HIS HANDS</t>
+  </si>
+  <si>
+    <t>HIGHER GROUND</t>
+  </si>
+  <si>
+    <t>HIS EYE IS ON THE SPARROW</t>
+  </si>
+  <si>
+    <t>HOLY HOLY HOLY</t>
+  </si>
+  <si>
+    <t>HOW GREAT THOU ART</t>
+  </si>
+  <si>
+    <t>I AM THINE O LORD</t>
+  </si>
+  <si>
+    <t>I HAVE DECIDED TO FOLLOW JESUS</t>
+  </si>
+  <si>
+    <t>I LOVE TO TELL THE STORY</t>
+  </si>
+  <si>
+    <t>I LOVE YOU LORD</t>
+  </si>
+  <si>
+    <t>I NEED THEE EVERY HOUR</t>
+  </si>
+  <si>
+    <t>I STAND AMAZED IN THE PRESENCE</t>
+  </si>
+  <si>
+    <t>I SURRENDER ALL</t>
+  </si>
+  <si>
+    <t>IMMORTAL INVISIBLE GOD ONLY WISE</t>
+  </si>
+  <si>
+    <t>IN THE GARDEN</t>
+  </si>
+  <si>
+    <t>IN THE SWEET BY AND BY</t>
+  </si>
+  <si>
+    <t>IT IS WELL WITH MY SOUL</t>
+  </si>
+  <si>
+    <t>I'VE GOT PEACE LIKE A RIVER</t>
+  </si>
+  <si>
+    <t>JESUS KEEP ME NEAR THE CROSS</t>
+  </si>
+  <si>
+    <t>JESUS LOVES ME</t>
+  </si>
+  <si>
+    <t>JESUS PAID IT ALL</t>
+  </si>
+  <si>
+    <t>JESUS WHAT A FRIEND FOR SINNERS</t>
+  </si>
+  <si>
+    <t>JESUS SAVES</t>
+  </si>
+  <si>
+    <t>JOYFUL JOYFUL WE ADORE THEE</t>
+  </si>
+  <si>
+    <t>JUST A CLOSER WALK WITH THEE</t>
+  </si>
+  <si>
+    <t>JUST AS I AM</t>
+  </si>
+  <si>
+    <t>LEANING ON THE EVERLASTING ARMS</t>
+  </si>
+  <si>
+    <t>LET US BREAK BREAD TOGETHER</t>
+  </si>
+  <si>
+    <t>LOW IN THE GRAVE HE LAY</t>
+  </si>
+  <si>
+    <t>MY FAITH HAS FOUND A RESTING PLACE</t>
+  </si>
+  <si>
+    <t>MY JESUS I LOVE THEE</t>
+  </si>
+  <si>
+    <t>NEAR TO THE HEART OF GOD</t>
+  </si>
+  <si>
+    <t>NO NOT ONE</t>
+  </si>
+  <si>
+    <t>NOTHING BUT THE BLOOD</t>
+  </si>
+  <si>
+    <t>O FOR A THOUSAND TONGUES TO SING BLESSED BE THE NAME</t>
+  </si>
+  <si>
+    <t>O HOW HE LOVES YOU AND ME</t>
+  </si>
+  <si>
+    <t>O WORSHIP THE KING</t>
+  </si>
+  <si>
+    <t>O HOW I LOVE JESUS</t>
+  </si>
+  <si>
+    <t>OPEN MY EYES THAT I MAY SEE</t>
+  </si>
+  <si>
+    <t>OPEN OUR EYES LORD</t>
+  </si>
+  <si>
+    <t>PRAISE HIM PRAISE HIM</t>
+  </si>
+  <si>
+    <t>PRAISE TO THE LORD THE ALMIGHTY</t>
+  </si>
+  <si>
+    <t>PRECIOUS LORD TAKE MY HAND</t>
+  </si>
+  <si>
+    <t>REJOICE IN THE LORD ALWAYS</t>
+  </si>
+  <si>
+    <t>REVIVE US AGAIN</t>
+  </si>
+  <si>
+    <t>ROCK OF AGES CLEFT FOR ME</t>
+  </si>
+  <si>
+    <t>SAVIOR LIKE A SHEPHERD LEAD US</t>
+  </si>
+  <si>
+    <t>SHALL WE GATHER AT THE RIVER</t>
+  </si>
+  <si>
+    <t>SINCE JESUS CAME INTO MY HEART</t>
+  </si>
+  <si>
+    <t>SOFTLY AND TENDERLY</t>
+  </si>
+  <si>
+    <t>STANDING ON THE PROMISES</t>
+  </si>
+  <si>
+    <t>SWEET HOUR OF PRAYER</t>
+  </si>
+  <si>
+    <t>TAKE MY LIFE AND LET IT BE CONSECRATED</t>
+  </si>
+  <si>
+    <t>THE OLD RUGGED CROSS</t>
+  </si>
+  <si>
+    <t>THE SOLID ROCK MY HOPE IS BUILT</t>
+  </si>
+  <si>
+    <t>THERE IS A FOUNTAIN</t>
+  </si>
+  <si>
+    <t>THERE IS POWER IN THE BLOOD</t>
+  </si>
+  <si>
+    <t>TIS SO SWEET TO TRUST IN JESUS</t>
+  </si>
+  <si>
+    <t>TO GOD BE THE GLORY</t>
+  </si>
+  <si>
+    <t>TRUST AND OBEY</t>
+  </si>
+  <si>
+    <t>TURN YOUR EYES UPON JESUS</t>
+  </si>
+  <si>
+    <t>VICTORY IN JESUS</t>
+  </si>
+  <si>
+    <t>WERE YOU THERE</t>
+  </si>
+  <si>
+    <t>WHAT A FRIEND WE HAVE IN JESUS</t>
+  </si>
+  <si>
+    <t>WHAT WONDROUS LOVE IS THIS</t>
+  </si>
+  <si>
+    <t>WHEN I SURVEY THE WONDROUS CROSS</t>
+  </si>
+  <si>
+    <t>WHEN THE MORNING COMES</t>
+  </si>
+  <si>
+    <t>WHEN THE ROLL IS CALLED UP YONDER</t>
+  </si>
+  <si>
+    <t>WHEN WE ALL GET TO HEAVEN</t>
+  </si>
+  <si>
+    <t>Be Still, For The Presence Of The Lord</t>
+  </si>
+  <si>
+    <t>Dear Lord And Father Of Mankind</t>
+  </si>
+  <si>
+    <t>Here I Am, Lord (I, The Lord Of Sea And Sky)</t>
+  </si>
+  <si>
+    <t>And Can It Be</t>
+  </si>
+  <si>
+    <t>Guide Me, O Thou Great Redeemer/Jehova</t>
+  </si>
+  <si>
+    <t>Make Me A Channel Of Your Peace</t>
+  </si>
+  <si>
+    <t>The Day Thou Gavest, Lord, Is Ended</t>
+  </si>
+  <si>
+    <t>Jerusalem</t>
+  </si>
+  <si>
+    <t>Shine Jesus Shine (Lord, The Light Of Your Love Is Shining)</t>
+  </si>
+  <si>
+    <t>Love Divine, All Love Excelling</t>
+  </si>
+  <si>
+    <t>I Vow To Thee My Country</t>
+  </si>
+  <si>
+    <t>When I Survey the Wondrous Cross</t>
+  </si>
+  <si>
+    <t>What A Friend We have In Jesus</t>
+  </si>
+  <si>
+    <t>Thine Be The Glory</t>
+  </si>
+  <si>
+    <t>To God Be The Glory</t>
+  </si>
+  <si>
+    <t>Praise, My Soul, The King Of Heaven</t>
+  </si>
+  <si>
+    <t>Be Still, My Soul</t>
+  </si>
+  <si>
+    <t>How Deep The Father’s Love For Us</t>
+  </si>
+  <si>
+    <t>Will Your Anchor Hold In The Storms Of Life</t>
+  </si>
+  <si>
+    <t>Psalm 23 (by Stuart Townend)</t>
+  </si>
+  <si>
+    <t>O Love That Wilt Not Let Me Go</t>
+  </si>
+  <si>
+    <t>Lord, For The Years</t>
+  </si>
+  <si>
+    <t>Lord Of All Hopefulness</t>
+  </si>
+  <si>
+    <t>O Jesus, I Have Promised</t>
+  </si>
+  <si>
+    <t>All Things Bright And Beautiful</t>
+  </si>
+  <si>
+    <t>The Lord's My Shepherd, I'll Not Want</t>
+  </si>
+  <si>
+    <t>King Of Kings, Majesty</t>
+  </si>
+  <si>
+    <t>Beauty For Brokenness</t>
+  </si>
+  <si>
+    <t>Lord Of The Dance</t>
+  </si>
+  <si>
+    <t>My Song Is Love Unknown</t>
+  </si>
+  <si>
+    <t>My Jesus, My Saviour</t>
+  </si>
+  <si>
+    <t>Here I Am To Worship (Light Of The World)</t>
+  </si>
+  <si>
+    <t>Immortal, Invisible, God Only Wise</t>
+  </si>
+  <si>
+    <t>Angel-Voices Ever Singing</t>
+  </si>
+  <si>
+    <t>Before The Throne Of God</t>
+  </si>
+  <si>
+    <t>Here Is Love, Vast As The Ocean</t>
+  </si>
+  <si>
+    <t>The King Of Love My Shepherd Is</t>
+  </si>
+  <si>
+    <t>At The Name Of Jesus</t>
+  </si>
+  <si>
+    <t>Brother, Let Me Be Your Servant</t>
+  </si>
+  <si>
+    <t>I’ll Go In The Strength Of The Lord</t>
+  </si>
+  <si>
+    <t>Soul Of My Saviour</t>
+  </si>
+  <si>
+    <t>Christ Triumphant, Ever Reigning</t>
+  </si>
+  <si>
+    <t>For All The Saints</t>
+  </si>
+  <si>
+    <t>O Happy Day</t>
+  </si>
+  <si>
+    <t>The Church’s One Foundation</t>
+  </si>
+  <si>
+    <t>He Who Would Valiant Be</t>
+  </si>
+  <si>
+    <t>How Shall I Sing That Majesty</t>
+  </si>
+  <si>
+    <t>Take My Life</t>
+  </si>
+  <si>
+    <t>Mine Eyes have Seen The Glory</t>
+  </si>
+  <si>
+    <t>I Will Sing The Wondrous Story</t>
+  </si>
+  <si>
+    <t>Now Thank We All Our God</t>
+  </si>
+  <si>
+    <t>There’s A Wideness In God’s Mercy</t>
+  </si>
+  <si>
+    <t>Holy, Holy, Holy, Lord God Almighty</t>
+  </si>
+  <si>
+    <t>Come Down, O Love Divine</t>
+  </si>
+  <si>
+    <t>Who Would True Valour See</t>
+  </si>
+  <si>
+    <t>Father, Hear The Prayer We Offer</t>
+  </si>
+  <si>
+    <t>All My Hope On God Is Founded</t>
+  </si>
+  <si>
+    <t>Lead Us, Heavenly Father</t>
+  </si>
+  <si>
+    <t>Christ Be Our Light</t>
+  </si>
+  <si>
+    <t>For The Beauty Of The Earth</t>
+  </si>
+  <si>
+    <t>Christ Is Made The Sure Foundation</t>
+  </si>
+  <si>
+    <t>Thy Hand, O God, Has Guided</t>
+  </si>
+  <si>
+    <t>Since Jesus Came Into My Heart</t>
+  </si>
+  <si>
+    <t>We Cannot Measure How You Heal</t>
+  </si>
+  <si>
+    <t>Praise To The Lord, The Almighty</t>
+  </si>
+  <si>
+    <t>Ye Servants Of God</t>
+  </si>
+  <si>
+    <t>O God, Our Help In Ages Past</t>
+  </si>
+  <si>
+    <t>Praise To The Holiest In The Height</t>
+  </si>
+  <si>
+    <t>O Worship The King All Glorious Above</t>
+  </si>
+  <si>
+    <t>Like A Mighty River Flowing</t>
+  </si>
+  <si>
+    <t>Lord, Enthroned In Heavenly Splendour</t>
+  </si>
+  <si>
+    <t>Sing Of The Lord’s Goodness</t>
+  </si>
+  <si>
+    <t>O When The Saints</t>
+  </si>
+  <si>
+    <t>God Is Love, Let Heaven Adore Him</t>
+  </si>
+  <si>
+    <t>In Heavenly Love Abiding</t>
+  </si>
+  <si>
+    <t>Nearer My God To Thee</t>
+  </si>
+  <si>
+    <t>Lord, Jesus Christ (Living Lord)</t>
+  </si>
+  <si>
+    <t>Give Me Joy In My Heart</t>
+  </si>
+  <si>
+    <t>All People That On Earth Do Dwell</t>
+  </si>
+  <si>
+    <t>I Cannot Tell</t>
+  </si>
+  <si>
+    <t>Lead Kindly Light</t>
+  </si>
+  <si>
+    <t>All Creatures Of Our God And King</t>
+  </si>
+  <si>
+    <t>Hail, Redeemer, King Divine</t>
+  </si>
+  <si>
+    <t>Let All The World In Every Corner Sing</t>
+  </si>
+  <si>
+    <t>CCLI#</t>
+  </si>
+  <si>
+    <t>Crown Him with Many Crowns</t>
+  </si>
+  <si>
+    <t>All Creatures of Our God and King</t>
+  </si>
+  <si>
+    <t>It Is Well with My Soul</t>
+  </si>
+  <si>
+    <t>To God Be the Glory</t>
+  </si>
+  <si>
+    <t>Amazing Grace! How Sweet the Sound</t>
+  </si>
+  <si>
+    <t>Come, Thou Fount of Every Blessing</t>
+  </si>
+  <si>
+    <t>Blessed Assurance, Jesus Is Mine</t>
+  </si>
+  <si>
+    <t>In Christ Alone (My Hope Is Found)</t>
+  </si>
+  <si>
+    <t>All Hail the Power of Jesus' Name</t>
+  </si>
+  <si>
+    <t>Victory in Jesus</t>
+  </si>
+  <si>
+    <t>I Stand Amazed in the Presence</t>
+  </si>
+  <si>
+    <t>A Mighty Fortress is Our God</t>
+  </si>
+  <si>
+    <t>Wherever He Leads I'll Go</t>
+  </si>
+  <si>
+    <t>Tis So Sweet to Trust in Jesus</t>
+  </si>
+  <si>
+    <t>Joyful, Joyful, We Adore Thee</t>
+  </si>
+  <si>
+    <t>Worthy of Worship</t>
+  </si>
+  <si>
+    <t>At the Cross</t>
+  </si>
+  <si>
+    <t>When We All Get to Heaven</t>
+  </si>
+  <si>
+    <t>He Keeps Me Singing</t>
+  </si>
+  <si>
+    <t>The Love of God</t>
+  </si>
+  <si>
+    <t>Nothing but the Blood</t>
+  </si>
+  <si>
+    <t>Grace Greater Than Our Sin</t>
+  </si>
+  <si>
+    <t>My Jesus, I Love Thee</t>
+  </si>
+  <si>
+    <t>Praise to the Lord, the Almighty</t>
+  </si>
+  <si>
+    <t>Turn Your Eyes upon Jesus</t>
+  </si>
+  <si>
+    <t>What a Friend We Have in Jesus</t>
+  </si>
+  <si>
+    <t>O God, Our Help in Ages Past</t>
+  </si>
+  <si>
+    <t>Jesus! What a Friend for Sinners</t>
+  </si>
+  <si>
+    <t>Brethren, We Have Met to Worship</t>
+  </si>
+  <si>
+    <t>O Worship the King</t>
+  </si>
+  <si>
+    <t>There Is Power in the Blood</t>
+  </si>
+  <si>
+    <t>Christ Arose</t>
+  </si>
+  <si>
+    <t>There Is a Fountain</t>
+  </si>
+  <si>
+    <t>Heaven Came Down</t>
+  </si>
+  <si>
+    <t>Come, Thou Almighty King</t>
+  </si>
+  <si>
+    <t>Trust and Obey</t>
+  </si>
+  <si>
+    <t>Are You Washed in the Blood</t>
+  </si>
+  <si>
+    <t>Rejoice, the Lord Is King</t>
+  </si>
+  <si>
+    <t>I Need Thee Every Hour</t>
+  </si>
+  <si>
+    <t>Christ the Lord Is Risen Today</t>
+  </si>
+  <si>
+    <t>How Deep the Father's Love</t>
+  </si>
+  <si>
+    <t>The Solid Rock</t>
+  </si>
+  <si>
+    <t>Since Jesus Came into My Heart</t>
+  </si>
+  <si>
+    <t>I Have Decided to Follow Jesus</t>
+  </si>
+  <si>
+    <t>Wonderful Grace of Jesus</t>
+  </si>
+  <si>
+    <t>O Church, Arise</t>
+  </si>
+  <si>
+    <t>Down at the Cross</t>
+  </si>
+  <si>
+    <t>Glorious Is Thy Name</t>
+  </si>
+  <si>
+    <t>Oh, How I Love Jesus</t>
+  </si>
+  <si>
+    <t>Speak, O Lord</t>
+  </si>
+  <si>
+    <t>Higher Ground</t>
+  </si>
+  <si>
+    <t>The Church's One Foundation</t>
+  </si>
+  <si>
+    <t>How Firm a Foundation</t>
+  </si>
+  <si>
+    <t>What a Day That Will Be</t>
+  </si>
+  <si>
+    <t>I Know Whom I Have Believed</t>
+  </si>
+  <si>
+    <t>Blessed Be the Name</t>
+  </si>
+  <si>
+    <t>Oh, How He Loves You and Me</t>
+  </si>
+  <si>
+    <t>I Love to Tell the Story</t>
+  </si>
+  <si>
+    <t>Come, Ye Thankful People, Come</t>
+  </si>
+  <si>
+    <t>Send the Light</t>
+  </si>
+  <si>
+    <t>Come, Christians, Join to Sing</t>
+  </si>
+  <si>
+    <t>We Have Heard the Joyful Sound</t>
+  </si>
+  <si>
+    <t>He Is Lord</t>
+  </si>
+  <si>
+    <t>Stand Up, Stand Up for Jesus</t>
+  </si>
+  <si>
+    <t>The Blood Will Never Lose Its Power</t>
+  </si>
+  <si>
+    <t>I Will Sing of My Redeemer</t>
+  </si>
+  <si>
+    <t>Just a Closer Walk with Thee</t>
+  </si>
+  <si>
+    <t>Lamb of God</t>
+  </si>
+  <si>
+    <t>His Eye Is On The Sparrow</t>
+  </si>
+  <si>
+    <t>When the Roll Is Called up Yonder</t>
+  </si>
+  <si>
+    <t>Redeemed, How I Love to Proclaim It</t>
+  </si>
+  <si>
+    <t>A New Name in Glory</t>
+  </si>
+  <si>
+    <t>The Communion Hymn (Behold the Lamb)</t>
   </si>
 </sst>
 </file>
@@ -1827,10 +2895,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4254,7 +5323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E7E1EC-4820-4514-A89A-322361245AE5}">
   <dimension ref="A1:H196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -9087,6 +10156,1049 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F196">
     <sortCondition ref="B2:B196"/>
   </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DC0E23-DF2D-4D47-AF7C-9304DB940264}">
+  <dimension ref="A1:A101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>772</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4403939-657E-4A97-9AB2-0A8AECFF6957}">
+  <dimension ref="A1:B101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>930</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B101" xr:uid="{29101994-D330-4E1C-A633-D018330C5613}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -23108,4 +25220,1057 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D229211C-7705-4513-A268-CE5F14037AAA}">
+  <dimension ref="A1:I101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>857</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>846</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:B101" xr:uid="{18151449-F1F0-4404-95DB-F9C70E6F844B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225690FD-D426-4689-B77D-F5DA06A561A8}">
+  <dimension ref="A1:I101"/>
+  <sheetViews>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>579</v>
+      </c>
+      <c r="I2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>672</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned data in Passion, WowWorship, CcliTop100-Hymns.
</commit_message>
<xml_diff>
--- a/WorshipCreator.TestData/Source/Books/CcliTop100/CcliTop100.xlsx
+++ b/WorshipCreator.TestData/Source/Books/CcliTop100/CcliTop100.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PageOptimizer\Data\WorshipCreator.TestData\Source\Books\CcliTop100\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06632916-C13B-4981-B5C6-055AEC3B70B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23811ECA-5973-4357-8335-BB63278E4E93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5280" yWindow="4245" windowWidth="21600" windowHeight="11505" firstSheet="5" activeTab="10" xr2:uid="{8764540B-17CA-4663-B848-BB803B99CCC3}"/>
+    <workbookView xWindow="3990" yWindow="2535" windowWidth="21600" windowHeight="11505" firstSheet="6" activeTab="9" xr2:uid="{8764540B-17CA-4663-B848-BB803B99CCC3}"/>
   </bookViews>
   <sheets>
     <sheet name="CcliCombined" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Top100HymnsBBC" sheetId="8" r:id="rId8"/>
     <sheet name="Top100HymnsPopularHymns" sheetId="9" r:id="rId9"/>
     <sheet name="Top100HymnsJWPepper" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet4" sheetId="11" r:id="rId11"/>
+    <sheet name="Top100HymnsLifewayWorship" sheetId="11" r:id="rId11"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId12"/>
@@ -37,8 +37,10 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">MultiTracksTop120!$A$1:$F$121</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">MultiTracksTop120Global!$A$1:$F$121</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">PraiseChartsTop100AllTime!$A$1:$H$100</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Sheet4!$A$1:$B$101</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Top100HymnsBBC!$A$1:$B$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Top100HymnsJWPepper!$A$1:$B$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Top100HymnsLifewayWorship!$A$1:$B$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Top100HymnsPopularHymns!$A$1:$B$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2973" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2977" uniqueCount="888">
   <si>
     <t>Way Maker</t>
   </si>
@@ -2080,306 +2082,6 @@
     <t>Yesterday, Today, Forever</t>
   </si>
   <si>
-    <t>A MIGHTY FORTRESS IS OUR GOD</t>
-  </si>
-  <si>
-    <t>ABIDE WITH ME</t>
-  </si>
-  <si>
-    <t>ALL CREATURES OF OUR GOD AND KING</t>
-  </si>
-  <si>
-    <t>ALL HAIL THE POWER OF JESUS NAME</t>
-  </si>
-  <si>
-    <t>AMAZING GRACE</t>
-  </si>
-  <si>
-    <t>AND CAN IT BE</t>
-  </si>
-  <si>
-    <t>ARE YOU WASHED IN THE BLOOD</t>
-  </si>
-  <si>
-    <t>AT THE CROSS</t>
-  </si>
-  <si>
-    <t>BE THOU MY VISION</t>
-  </si>
-  <si>
-    <t>BECAUSE HE LIVES</t>
-  </si>
-  <si>
-    <t>BLESS THE LORD O MY SOUL</t>
-  </si>
-  <si>
-    <t>BLESSED ASSURANCE</t>
-  </si>
-  <si>
-    <t>BREATHE ON ME BREATH OF GOD</t>
-  </si>
-  <si>
-    <t>CHRIST THE LORD IS RISEN TODAY</t>
-  </si>
-  <si>
-    <t>COME THOU ALMIGHTY KING</t>
-  </si>
-  <si>
-    <t>COME THOU FOUNT OF EVERY BLESSING</t>
-  </si>
-  <si>
-    <t>COUNT YOUR BLESSINGS</t>
-  </si>
-  <si>
-    <t>CROWN HIM WITH MANY CROWNS</t>
-  </si>
-  <si>
-    <t>DOWN AT THE CROSS</t>
-  </si>
-  <si>
-    <t>DOXOLOGY</t>
-  </si>
-  <si>
-    <t>FAIREST LORD JESUS</t>
-  </si>
-  <si>
-    <t>FATHER I ADORE YOU</t>
-  </si>
-  <si>
-    <t>GLORIFY THY NAME</t>
-  </si>
-  <si>
-    <t>GOD WILL TAKE CARE OF YOU</t>
-  </si>
-  <si>
-    <t>GRACE GREATER THAN OUR SIN</t>
-  </si>
-  <si>
-    <t>GREAT IS THY FAITHFULNESS</t>
-  </si>
-  <si>
-    <t>HALLELUJAH WHAT A SAVIOR</t>
-  </si>
-  <si>
-    <t>HAVE THINE OWN WAY LORD</t>
-  </si>
-  <si>
-    <t>HE HIDETH MY SOUL</t>
-  </si>
-  <si>
-    <t>HE KEEPS ME SINGING</t>
-  </si>
-  <si>
-    <t>HE LIVES</t>
-  </si>
-  <si>
-    <t>HEAVEN CAME DOWN</t>
-  </si>
-  <si>
-    <t>HE'S GOT THE WHOLE WORLD IN HIS HANDS</t>
-  </si>
-  <si>
-    <t>HIGHER GROUND</t>
-  </si>
-  <si>
-    <t>HIS EYE IS ON THE SPARROW</t>
-  </si>
-  <si>
-    <t>HOLY HOLY HOLY</t>
-  </si>
-  <si>
-    <t>HOW GREAT THOU ART</t>
-  </si>
-  <si>
-    <t>I AM THINE O LORD</t>
-  </si>
-  <si>
-    <t>I HAVE DECIDED TO FOLLOW JESUS</t>
-  </si>
-  <si>
-    <t>I LOVE TO TELL THE STORY</t>
-  </si>
-  <si>
-    <t>I LOVE YOU LORD</t>
-  </si>
-  <si>
-    <t>I NEED THEE EVERY HOUR</t>
-  </si>
-  <si>
-    <t>I STAND AMAZED IN THE PRESENCE</t>
-  </si>
-  <si>
-    <t>I SURRENDER ALL</t>
-  </si>
-  <si>
-    <t>IMMORTAL INVISIBLE GOD ONLY WISE</t>
-  </si>
-  <si>
-    <t>IN THE GARDEN</t>
-  </si>
-  <si>
-    <t>IN THE SWEET BY AND BY</t>
-  </si>
-  <si>
-    <t>IT IS WELL WITH MY SOUL</t>
-  </si>
-  <si>
-    <t>I'VE GOT PEACE LIKE A RIVER</t>
-  </si>
-  <si>
-    <t>JESUS KEEP ME NEAR THE CROSS</t>
-  </si>
-  <si>
-    <t>JESUS LOVES ME</t>
-  </si>
-  <si>
-    <t>JESUS PAID IT ALL</t>
-  </si>
-  <si>
-    <t>JESUS WHAT A FRIEND FOR SINNERS</t>
-  </si>
-  <si>
-    <t>JESUS SAVES</t>
-  </si>
-  <si>
-    <t>JOYFUL JOYFUL WE ADORE THEE</t>
-  </si>
-  <si>
-    <t>JUST A CLOSER WALK WITH THEE</t>
-  </si>
-  <si>
-    <t>JUST AS I AM</t>
-  </si>
-  <si>
-    <t>LEANING ON THE EVERLASTING ARMS</t>
-  </si>
-  <si>
-    <t>LET US BREAK BREAD TOGETHER</t>
-  </si>
-  <si>
-    <t>LOW IN THE GRAVE HE LAY</t>
-  </si>
-  <si>
-    <t>MY FAITH HAS FOUND A RESTING PLACE</t>
-  </si>
-  <si>
-    <t>MY JESUS I LOVE THEE</t>
-  </si>
-  <si>
-    <t>NEAR TO THE HEART OF GOD</t>
-  </si>
-  <si>
-    <t>NO NOT ONE</t>
-  </si>
-  <si>
-    <t>NOTHING BUT THE BLOOD</t>
-  </si>
-  <si>
-    <t>O FOR A THOUSAND TONGUES TO SING BLESSED BE THE NAME</t>
-  </si>
-  <si>
-    <t>O HOW HE LOVES YOU AND ME</t>
-  </si>
-  <si>
-    <t>O WORSHIP THE KING</t>
-  </si>
-  <si>
-    <t>O HOW I LOVE JESUS</t>
-  </si>
-  <si>
-    <t>OPEN MY EYES THAT I MAY SEE</t>
-  </si>
-  <si>
-    <t>OPEN OUR EYES LORD</t>
-  </si>
-  <si>
-    <t>PRAISE HIM PRAISE HIM</t>
-  </si>
-  <si>
-    <t>PRAISE TO THE LORD THE ALMIGHTY</t>
-  </si>
-  <si>
-    <t>PRECIOUS LORD TAKE MY HAND</t>
-  </si>
-  <si>
-    <t>REJOICE IN THE LORD ALWAYS</t>
-  </si>
-  <si>
-    <t>REVIVE US AGAIN</t>
-  </si>
-  <si>
-    <t>ROCK OF AGES CLEFT FOR ME</t>
-  </si>
-  <si>
-    <t>SAVIOR LIKE A SHEPHERD LEAD US</t>
-  </si>
-  <si>
-    <t>SHALL WE GATHER AT THE RIVER</t>
-  </si>
-  <si>
-    <t>SINCE JESUS CAME INTO MY HEART</t>
-  </si>
-  <si>
-    <t>SOFTLY AND TENDERLY</t>
-  </si>
-  <si>
-    <t>STANDING ON THE PROMISES</t>
-  </si>
-  <si>
-    <t>SWEET HOUR OF PRAYER</t>
-  </si>
-  <si>
-    <t>TAKE MY LIFE AND LET IT BE CONSECRATED</t>
-  </si>
-  <si>
-    <t>THE OLD RUGGED CROSS</t>
-  </si>
-  <si>
-    <t>THE SOLID ROCK MY HOPE IS BUILT</t>
-  </si>
-  <si>
-    <t>THERE IS A FOUNTAIN</t>
-  </si>
-  <si>
-    <t>THERE IS POWER IN THE BLOOD</t>
-  </si>
-  <si>
-    <t>TIS SO SWEET TO TRUST IN JESUS</t>
-  </si>
-  <si>
-    <t>TO GOD BE THE GLORY</t>
-  </si>
-  <si>
-    <t>TRUST AND OBEY</t>
-  </si>
-  <si>
-    <t>TURN YOUR EYES UPON JESUS</t>
-  </si>
-  <si>
-    <t>VICTORY IN JESUS</t>
-  </si>
-  <si>
-    <t>WERE YOU THERE</t>
-  </si>
-  <si>
-    <t>WHAT A FRIEND WE HAVE IN JESUS</t>
-  </si>
-  <si>
-    <t>WHAT WONDROUS LOVE IS THIS</t>
-  </si>
-  <si>
-    <t>WHEN I SURVEY THE WONDROUS CROSS</t>
-  </si>
-  <si>
-    <t>WHEN THE MORNING COMES</t>
-  </si>
-  <si>
-    <t>WHEN THE ROLL IS CALLED UP YONDER</t>
-  </si>
-  <si>
-    <t>WHEN WE ALL GET TO HEAVEN</t>
-  </si>
-  <si>
     <t>Be Still, For The Presence Of The Lord</t>
   </si>
   <si>
@@ -2852,13 +2554,184 @@
   </si>
   <si>
     <t>The Communion Hymn (Behold the Lamb)</t>
+  </si>
+  <si>
+    <t>https://genius.com/albums/Lifeway-worship/Top-100-hymns</t>
+  </si>
+  <si>
+    <t>https://www.jwpepper.com/Top-100-Hymns-Guitar-Songbook/10089160.item#/submit</t>
+  </si>
+  <si>
+    <t>All Hail The Power Of Jesus Name</t>
+  </si>
+  <si>
+    <t>Are You Washed In The Blood</t>
+  </si>
+  <si>
+    <t>Bless The Lord O My Soul</t>
+  </si>
+  <si>
+    <t>Breathe On Me Breath Of God</t>
+  </si>
+  <si>
+    <t>Come Thou Almighty King</t>
+  </si>
+  <si>
+    <t>Come Thou Fount Of Every Blessing</t>
+  </si>
+  <si>
+    <t>Down At The Cross</t>
+  </si>
+  <si>
+    <t>Father I Adore You</t>
+  </si>
+  <si>
+    <t>Glorify Thy Name</t>
+  </si>
+  <si>
+    <t>Hallelujah What A Savior</t>
+  </si>
+  <si>
+    <t>Have Thine Own Way Lord</t>
+  </si>
+  <si>
+    <t>He's Got The Whole World In His Hands</t>
+  </si>
+  <si>
+    <t>Holy Holy Holy</t>
+  </si>
+  <si>
+    <t>I Am Thine O Lord</t>
+  </si>
+  <si>
+    <t>I Have Decided To Follow Jesus</t>
+  </si>
+  <si>
+    <t>I Love You Lord</t>
+  </si>
+  <si>
+    <t>I Stand Amazed In The Presence</t>
+  </si>
+  <si>
+    <t>Immortal Invisible God Only Wise</t>
+  </si>
+  <si>
+    <t>In The Garden</t>
+  </si>
+  <si>
+    <t>In The Sweet By And By</t>
+  </si>
+  <si>
+    <t>It Is Well With My Soul</t>
+  </si>
+  <si>
+    <t>I've Got Peace Like A River</t>
+  </si>
+  <si>
+    <t>Jesus Keep Me Near The Cross</t>
+  </si>
+  <si>
+    <t>Jesus What A Friend For Sinners</t>
+  </si>
+  <si>
+    <t>Jesus Saves</t>
+  </si>
+  <si>
+    <t>Joyful Joyful We Adore Thee</t>
+  </si>
+  <si>
+    <t>Just A Closer Walk With Thee</t>
+  </si>
+  <si>
+    <t>Leaning On The Everlasting Arms</t>
+  </si>
+  <si>
+    <t>Let Us Break Bread Together</t>
+  </si>
+  <si>
+    <t>Low In The Grave He Lay</t>
+  </si>
+  <si>
+    <t>My Faith Has Found A Resting Place</t>
+  </si>
+  <si>
+    <t>My Jesus I Love Thee</t>
+  </si>
+  <si>
+    <t>Near To The Heart Of God</t>
+  </si>
+  <si>
+    <t>No Not One</t>
+  </si>
+  <si>
+    <t>Nothing But The Blood</t>
+  </si>
+  <si>
+    <t>O How He Loves You And Me</t>
+  </si>
+  <si>
+    <t>O How I Love Jesus</t>
+  </si>
+  <si>
+    <t>Open My Eyes That I May See</t>
+  </si>
+  <si>
+    <t>Open Our Eyes Lord</t>
+  </si>
+  <si>
+    <t>Praise Him Praise Him</t>
+  </si>
+  <si>
+    <t>Praise To The Lord The Almighty</t>
+  </si>
+  <si>
+    <t>Rejoice In The Lord Always</t>
+  </si>
+  <si>
+    <t>Rock Of Ages Cleft For Me</t>
+  </si>
+  <si>
+    <t>Savior Like A Shepherd Lead Us</t>
+  </si>
+  <si>
+    <t>Shall We Gather At The River</t>
+  </si>
+  <si>
+    <t>Softly And Tenderly</t>
+  </si>
+  <si>
+    <t>Standing On The Promises</t>
+  </si>
+  <si>
+    <t>Sweet Hour Of Prayer</t>
+  </si>
+  <si>
+    <t>Take My Life And Let It Be Consecrated</t>
+  </si>
+  <si>
+    <t>The Solid Rock My Hope Is Built</t>
+  </si>
+  <si>
+    <t>Tis So Sweet To Trust In Jesus</t>
+  </si>
+  <si>
+    <t>Were You There</t>
+  </si>
+  <si>
+    <t>What A Friend We Have In Jesus</t>
+  </si>
+  <si>
+    <t>What Wondrous Love Is This</t>
+  </si>
+  <si>
+    <t>When The Morning Comes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2870,6 +2743,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2895,11 +2775,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10162,639 +10045,658 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DC0E23-DF2D-4D47-AF7C-9304DB940264}">
-  <dimension ref="A1:A101"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B1" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>762</v>
-      </c>
-    </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>763</v>
+      <c r="A92" s="4" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>764</v>
+      <c r="A93" s="4" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>765</v>
+      <c r="A94" s="4" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>766</v>
+      <c r="A95" s="4" t="s">
+        <v>884</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>767</v>
+      <c r="A96" s="4" t="s">
+        <v>885</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>768</v>
+      <c r="A97" s="4" t="s">
+        <v>886</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>769</v>
+      <c r="A98" s="4" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>770</v>
+      <c r="A99" s="4" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>771</v>
+      <c r="A100" s="4" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>772</v>
+      <c r="A101" s="4" t="s">
+        <v>670</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B101" xr:uid="{BD903512-2044-45A5-8C56-7BCF1E75E31F}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4403939-657E-4A97-9AB2-0A8AECFF6957}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>274</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>757</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>868</v>
+        <v>768</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>869</v>
+        <v>769</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>870</v>
+        <v>770</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>871</v>
+        <v>771</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>872</v>
+        <v>772</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>873</v>
+        <v>773</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -10809,12 +10711,12 @@
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>874</v>
+        <v>774</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>875</v>
+        <v>775</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -10824,17 +10726,17 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>789</v>
+        <v>689</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>876</v>
+        <v>776</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>877</v>
+        <v>777</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -10844,12 +10746,12 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>784</v>
+        <v>684</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>776</v>
+        <v>676</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -10859,17 +10761,17 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>878</v>
+        <v>778</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>879</v>
+        <v>779</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>880</v>
+        <v>780</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
@@ -10879,7 +10781,7 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>881</v>
+        <v>781</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
@@ -10889,32 +10791,32 @@
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>882</v>
+        <v>782</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>883</v>
+        <v>783</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>884</v>
+        <v>784</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>885</v>
+        <v>785</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>886</v>
+        <v>786</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>887</v>
+        <v>787</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
@@ -10924,7 +10826,7 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>888</v>
+        <v>788</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
@@ -10944,27 +10846,27 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>889</v>
+        <v>789</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>890</v>
+        <v>790</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>891</v>
+        <v>791</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>892</v>
+        <v>792</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>893</v>
+        <v>793</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -10974,12 +10876,12 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>894</v>
+        <v>794</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>895</v>
+        <v>795</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
@@ -10989,37 +10891,37 @@
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>896</v>
+        <v>796</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>897</v>
+        <v>797</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>898</v>
+        <v>798</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>899</v>
+        <v>799</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>900</v>
+        <v>800</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>901</v>
+        <v>801</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>902</v>
+        <v>802</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
@@ -11029,7 +10931,7 @@
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>903</v>
+        <v>803</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
@@ -11039,7 +10941,7 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>904</v>
+        <v>804</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
@@ -11049,7 +10951,7 @@
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>905</v>
+        <v>805</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
@@ -11059,17 +10961,17 @@
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>906</v>
+        <v>806</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>907</v>
+        <v>807</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>908</v>
+        <v>808</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
@@ -11079,7 +10981,7 @@
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>909</v>
+        <v>809</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
@@ -11089,87 +10991,87 @@
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>910</v>
+        <v>810</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>911</v>
+        <v>811</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>912</v>
+        <v>812</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>913</v>
+        <v>813</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>914</v>
+        <v>814</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>915</v>
+        <v>815</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>916</v>
+        <v>816</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>917</v>
+        <v>817</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>918</v>
+        <v>818</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>919</v>
+        <v>819</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>920</v>
+        <v>820</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>921</v>
+        <v>821</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>922</v>
+        <v>822</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>923</v>
+        <v>823</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>924</v>
+        <v>824</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>925</v>
+        <v>825</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>926</v>
+        <v>826</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
@@ -11179,22 +11081,22 @@
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>927</v>
+        <v>827</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>928</v>
+        <v>828</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>929</v>
+        <v>829</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>930</v>
+        <v>830</v>
       </c>
     </row>
   </sheetData>
@@ -25240,7 +25142,7 @@
         <v>274</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>857</v>
+        <v>757</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>577</v>
@@ -25258,22 +25160,22 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>773</v>
+        <v>673</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>774</v>
+        <v>674</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>775</v>
+        <v>675</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>776</v>
+        <v>676</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -25283,22 +25185,22 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>777</v>
+        <v>677</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>778</v>
+        <v>678</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>779</v>
+        <v>679</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>780</v>
+        <v>680</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -25308,12 +25210,12 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>781</v>
+        <v>681</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>782</v>
+        <v>682</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -25328,67 +25230,67 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>783</v>
+        <v>683</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>784</v>
+        <v>684</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>785</v>
+        <v>685</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>786</v>
+        <v>686</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>787</v>
+        <v>687</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>788</v>
+        <v>688</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>789</v>
+        <v>689</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>790</v>
+        <v>690</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>791</v>
+        <v>691</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>792</v>
+        <v>692</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>793</v>
+        <v>693</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>794</v>
+        <v>694</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>795</v>
+        <v>695</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -25398,7 +25300,7 @@
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>796</v>
+        <v>696</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
@@ -25408,17 +25310,17 @@
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>797</v>
+        <v>697</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>798</v>
+        <v>698</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>799</v>
+        <v>699</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
@@ -25428,12 +25330,12 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>800</v>
+        <v>700</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>801</v>
+        <v>701</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
@@ -25443,12 +25345,12 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>802</v>
+        <v>702</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>803</v>
+        <v>703</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
@@ -25458,17 +25360,17 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>804</v>
+        <v>704</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>805</v>
+        <v>705</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>806</v>
+        <v>706</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
@@ -25478,12 +25380,12 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>807</v>
+        <v>707</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>808</v>
+        <v>708</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
@@ -25493,17 +25395,17 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>809</v>
+        <v>709</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>847</v>
+        <v>747</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>810</v>
+        <v>710</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
@@ -25513,67 +25415,67 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>848</v>
+        <v>748</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>849</v>
+        <v>749</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>850</v>
+        <v>750</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>811</v>
+        <v>711</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>812</v>
+        <v>712</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>813</v>
+        <v>713</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>814</v>
+        <v>714</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>815</v>
+        <v>715</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>851</v>
+        <v>751</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>816</v>
+        <v>716</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>817</v>
+        <v>717</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>818</v>
+        <v>718</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>852</v>
+        <v>752</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
@@ -25583,7 +25485,7 @@
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>819</v>
+        <v>719</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
@@ -25593,157 +25495,157 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>820</v>
+        <v>720</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>853</v>
+        <v>753</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>821</v>
+        <v>721</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>822</v>
+        <v>722</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>823</v>
+        <v>723</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>824</v>
+        <v>724</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>825</v>
+        <v>725</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>826</v>
+        <v>726</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>827</v>
+        <v>727</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>854</v>
+        <v>754</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>828</v>
+        <v>728</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>829</v>
+        <v>729</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>830</v>
+        <v>730</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>831</v>
+        <v>731</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>832</v>
+        <v>732</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>833</v>
+        <v>733</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>855</v>
+        <v>755</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>834</v>
+        <v>734</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>835</v>
+        <v>735</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>836</v>
+        <v>736</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>837</v>
+        <v>737</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>838</v>
+        <v>738</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>839</v>
+        <v>739</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>840</v>
+        <v>740</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>841</v>
+        <v>741</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>842</v>
+        <v>742</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>856</v>
+        <v>756</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>843</v>
+        <v>743</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>844</v>
+        <v>744</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>845</v>
+        <v>745</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>846</v>
+        <v>746</v>
       </c>
     </row>
   </sheetData>
@@ -25756,24 +25658,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225690FD-D426-4689-B77D-F5DA06A561A8}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>274</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>579</v>
       </c>
-      <c r="I2" t="s">
-        <v>578</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -26271,6 +26180,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B101" xr:uid="{BEB806BE-9530-459B-BDB7-0691C7476729}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>